<commit_message>
Completed test for calc_load_and_loc.
Finished basic testing calc_load_and_loc. Used basic functionality in excel to
generate correct answers for testing. Saved excel file for potential
future use or a user looking for more information. Updated other excel
files that were used to generate input for the calc_load_and_loc excel
file.

All tests successful.
</commit_message>
<xml_diff>
--- a/test/get_abs_axle_location.xlsx
+++ b/test/get_abs_axle_location.xlsx
@@ -47,10 +47,10 @@
     <t>abs axle location</t>
   </si>
   <si>
-    <t>rtl</t>
-  </si>
-  <si>
     <t>total spacing</t>
+  </si>
+  <si>
+    <t>ltr</t>
   </si>
 </sst>
 </file>
@@ -414,7 +414,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D5" sqref="D5:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,7 +433,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1">
-        <v>20</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -441,7 +441,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -455,7 +455,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -474,7 +474,7 @@
       </c>
       <c r="D5">
         <f>IF($C$3="ltr",$C$2-C5, $C$2+C5)</f>
-        <v>20</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -490,7 +490,7 @@
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D22" si="0">IF($C$3="ltr",$C$2-C6, $C$2+C6)</f>
-        <v>28</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -506,7 +506,7 @@
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -522,7 +522,7 @@
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -538,7 +538,7 @@
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -554,7 +554,7 @@
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -570,7 +570,7 @@
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>57</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -586,7 +586,7 @@
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>63</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -602,7 +602,7 @@
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>68</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -618,7 +618,7 @@
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>76</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -634,7 +634,7 @@
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>84</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -650,7 +650,7 @@
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>89</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -666,7 +666,7 @@
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>94</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -682,7 +682,7 @@
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>99</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -698,7 +698,7 @@
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>108</v>
+        <v>-13</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -714,7 +714,7 @@
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>113</v>
+        <v>-18</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -730,7 +730,7 @@
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
-        <v>119</v>
+        <v>-24</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -746,7 +746,7 @@
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
-        <v>124</v>
+        <v>-29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>